<commit_message>
支持传递空参数 完善Docker run 命令的支持 baseDockerContainer.xlsx 添加实例，使用 Docker 在Linux 下搭建 Gitlab,Redmine,Jenkins 服务 baseDockerContainer.png 简单图解，搭建之后如何登陆
</commit_message>
<xml_diff>
--- a/excel/dockerContainer/baseDockerContainer.xlsx
+++ b/excel/dockerContainer/baseDockerContainer.xlsx
@@ -5,11 +5,11 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiasy/Documents/sourceFrame/excelWorkFlow/excel/dockerContainer/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiasy/Documents/sourceFrame/pyWorkFlow/excel/dockerContainer/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="28340"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540"/>
   </bookViews>
   <sheets>
     <sheet name="pngTest" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="113">
   <si>
     <t>子脚本输出</t>
     <rPh sb="0" eb="1">
@@ -223,31 +223,6 @@
     <t>脚本描述</t>
   </si>
   <si>
-    <t>利用给定 镜像 创建 容器 映射端口</t>
-    <rPh sb="0" eb="1">
-      <t>li'yong</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>gei'ding</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>jing'xiang</t>
-    </rPh>
-    <rPh sb="8" eb="9">
-      <t>chuang'jian</t>
-    </rPh>
-    <rPh sb="11" eb="12">
-      <t>rong'qi</t>
-    </rPh>
-    <rPh sb="14" eb="15">
-      <t>ying'she</t>
-    </rPh>
-    <rPh sb="16" eb="17">
-      <t>duan'kou</t>
-    </rPh>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>脚本路径</t>
   </si>
   <si>
@@ -282,13 +257,6 @@
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
   <si>
-    <t>名称:版本 这样的格式&lt;&gt;</t>
-    <rPh sb="0" eb="13">
-      <t>min'bheng</t>
-    </rPh>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
     <t>容器名</t>
     <rPh sb="0" eb="1">
       <t>rogn'qi</t>
@@ -299,9 +267,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>containerName</t>
-  </si>
-  <si>
     <t>容器名称</t>
     <rPh sb="0" eb="1">
       <t>rong'qi</t>
@@ -313,7 +278,37 @@
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
   <si>
-    <t>端口映射列表</t>
+    <t>主机容器名</t>
+    <rPh sb="0" eb="1">
+      <t>wen'jian'jiaying'she</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>hostname</t>
+  </si>
+  <si>
+    <t>volume</t>
+  </si>
+  <si>
+    <t>publish</t>
+  </si>
+  <si>
+    <t>环境变量[数组]</t>
+    <rPh sb="0" eb="1">
+      <t>wen'jian'jiaying'she</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>共享文件夹设置[数组]</t>
+    <rPh sb="0" eb="1">
+      <t>wen'jian'jiaying'she</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>端口映射列表[数组]</t>
     <rPh sb="0" eb="1">
       <t>duan'kou</t>
     </rPh>
@@ -323,58 +318,436 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>mappingPorts</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>80:80</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>pm2 管理用</t>
-    <rPh sb="4" eb="5">
-      <t>guan'li</t>
-    </rPh>
-    <rPh sb="6" eb="7">
-      <t>yong</t>
-    </rPh>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>6379:6379</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>redis服务</t>
-    <rPh sb="5" eb="6">
-      <t>fu'wu</t>
-    </rPh>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>共享文件夹设置</t>
+    <t>重启模式</t>
     <rPh sb="0" eb="1">
       <t>wen'jian'jiaying'she</t>
     </rPh>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>mappingFolder</t>
+    <t>restart</t>
+  </si>
+  <si>
+    <t>restart</t>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
   <si>
-    <t>共享文件夹</t>
-    <rPh sb="0" eb="5">
-      <t>gong'xiang</t>
+    <t>名称:版本</t>
+    <rPh sb="0" eb="13">
+      <t>min'bheng</t>
     </rPh>
     <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>link</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>链接容器[数组]</t>
+    <rPh sb="0" eb="1">
+      <t>wen'jian'jiaying'she</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>off</t>
+  </si>
+  <si>
+    <t>运行容器设置模板，注意左侧Stage1下面的off，这样使得它不会被执行</t>
+    <rPh sb="0" eb="1">
+      <t>li'yong</t>
+    </rPh>
+    <rPh sb="570" eb="571">
+      <t>gei'ding</t>
+    </rPh>
+    <rPh sb="573" eb="574">
+      <t>jing'xiang</t>
+    </rPh>
+    <rPh sb="576" eb="577">
+      <t>chuang'jian</t>
+    </rPh>
+    <rPh sb="579" eb="580">
+      <t>rong'qi</t>
+    </rPh>
+    <rPh sb="582" eb="583">
+      <t>ying'she</t>
+    </rPh>
+    <rPh sb="584" eb="585">
+      <t>duan'kou</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>宿主机路径1 : 容器路径1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>宿主机端口1 : 容器端口1</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>容器名 : 关联键</t>
+    <rPh sb="0" eb="1">
+      <t>rong'qi</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">其他容器名 </t>
+    <rPh sb="0" eb="1">
+      <t>qi'ta</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否有宿主机权限</t>
+    <rPh sb="0" eb="2">
+      <t>shi'fou</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>privileged</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>always / on-failure:10 /不填写</t>
+    <rPh sb="0" eb="3">
+      <t>bu'tian'xie</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>true/false / 可以不填写</t>
+    <rPh sb="0" eb="2">
+      <t>ke'yi</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>GitLab搭建第一步，sql容器</t>
+    <rPh sb="0" eb="1">
+      <t>li'yong</t>
+    </rPh>
+    <rPh sb="728" eb="729">
+      <t>gei'ding</t>
+    </rPh>
+    <rPh sb="731" eb="732">
+      <t>jing'xiang</t>
+    </rPh>
+    <rPh sb="734" eb="735">
+      <t>chuang'jian</t>
+    </rPh>
+    <rPh sb="737" eb="738">
+      <t>rong'qi</t>
+    </rPh>
+    <rPh sb="740" eb="741">
+      <t>ying'she</t>
+    </rPh>
+    <rPh sb="742" eb="743">
+      <t>duan'kou</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">gitlab-postgresql </t>
+    <rPh sb="0" eb="1">
+      <t>rong'qi</t>
+    </rPh>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>sameersbn/postgresql:9.6-2</t>
+  </si>
+  <si>
+    <t>sameersbn/postgresql:9.6-2</t>
+    <rPh sb="0" eb="4">
+      <t>shi'yong</t>
+    </rPh>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>/srv/docker/gitlab/postgresql:/var/lib/postgresql</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>env</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>两边双引号有程序添加，这里就写值</t>
+    <rPh sb="0" eb="485">
+      <t>yin'hao</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>DB_NAME=gitlabhq_production</t>
+  </si>
+  <si>
+    <t>DB_USER=gitlab</t>
+  </si>
+  <si>
+    <t>DB_PASS=password</t>
+  </si>
+  <si>
+    <t>DB_EXTENSION=pg_trgm</t>
+  </si>
+  <si>
+    <t>Stage2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>gitlab-redis</t>
+  </si>
+  <si>
+    <t>sameersbn/redis:latest</t>
+  </si>
+  <si>
+    <t>/srv/docker/gitlab/redis:/var/lib/redis</t>
+  </si>
+  <si>
+    <t>GitLab搭建第二步，redis容器</t>
+    <rPh sb="0" eb="1">
+      <t>li'yong</t>
+    </rPh>
+    <rPh sb="825" eb="826">
+      <t>gei'ding</t>
+    </rPh>
+    <rPh sb="828" eb="829">
+      <t>jing'xiang</t>
+    </rPh>
+    <rPh sb="831" eb="832">
+      <t>chuang'jian</t>
+    </rPh>
+    <rPh sb="834" eb="835">
+      <t>rong'qi</t>
+    </rPh>
+    <rPh sb="837" eb="838">
+      <t>ying'she</t>
+    </rPh>
+    <rPh sb="839" eb="840">
+      <t>duan'kou</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>GitLab搭建第三步，gitlab</t>
+    <rPh sb="0" eb="1">
+      <t>li'yong</t>
+    </rPh>
+    <rPh sb="841" eb="842">
+      <t>gei'ding</t>
+    </rPh>
+    <rPh sb="844" eb="845">
+      <t>jing'xiang</t>
+    </rPh>
+    <rPh sb="847" eb="848">
+      <t>chuang'jian</t>
+    </rPh>
+    <rPh sb="850" eb="851">
+      <t>rong'qi</t>
+    </rPh>
+    <rPh sb="853" eb="854">
+      <t>ying'she</t>
+    </rPh>
+    <rPh sb="855" eb="856">
+      <t>duan'kou</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>gitlab</t>
+  </si>
+  <si>
+    <t>sameersbn/gitlab:10.6.1</t>
+  </si>
+  <si>
+    <t>gitlab-postgresql:postgresql</t>
+  </si>
+  <si>
+    <t>gitlab-redis:redisio</t>
+  </si>
+  <si>
+    <t>10022:22</t>
+  </si>
+  <si>
+    <t>10080:80</t>
+  </si>
+  <si>
+    <t>GITLAB_PORT=10080</t>
+  </si>
+  <si>
+    <t>GITLAB_SSH_PORT=10022</t>
+  </si>
+  <si>
+    <t>GITLAB_SECRETS_DB_KEY_BASE=long-and-random-alpha-numeric-string</t>
+  </si>
+  <si>
+    <t>GITLAB_SECRETS_SECRET_KEY_BASE=long-and-random-alpha-numeric-string</t>
+  </si>
+  <si>
+    <t>GITLAB_SECRETS_OTP_KEY_BASE=long-and-random-alpha-numeric-string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/srv/docker/gitlab/gitlab:/home/git/data </t>
+  </si>
+  <si>
+    <t>Stage3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>最好先下载镜像，否则会比较慢</t>
+    <rPh sb="0" eb="299">
+      <t>dai'mai</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stage4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Redmine搭建第一步，SQL</t>
+    <rPh sb="0" eb="1">
+      <t>li'yong</t>
+    </rPh>
+    <rPh sb="918" eb="919">
+      <t>gei'ding</t>
+    </rPh>
+    <rPh sb="921" eb="922">
+      <t>jing'xiang</t>
+    </rPh>
+    <rPh sb="924" eb="925">
+      <t>chuang'jian</t>
+    </rPh>
+    <rPh sb="927" eb="928">
+      <t>rong'qi</t>
+    </rPh>
+    <rPh sb="930" eb="931">
+      <t>ying'she</t>
+    </rPh>
+    <rPh sb="932" eb="933">
+      <t>duan'kou</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>postgresql-redmine</t>
+  </si>
+  <si>
+    <t>DB_NAME=redmine_production</t>
+  </si>
+  <si>
+    <t>DB_USER=redmine</t>
+  </si>
+  <si>
+    <t>/srv/docker/redmine/postgresql:/var/lib/postgresql</t>
+  </si>
+  <si>
+    <t>Stage5</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>sameersbn/redmine:3.4.4-2</t>
+  </si>
+  <si>
+    <t>REDMINE_PORT=10083</t>
+  </si>
+  <si>
+    <t>10083:80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postgresql-redmine:postgresql </t>
+  </si>
+  <si>
+    <t>redmine</t>
+  </si>
+  <si>
+    <t>Redmine搭建第二步，Redmine</t>
+    <rPh sb="0" eb="1">
+      <t>li'yong</t>
+    </rPh>
+    <rPh sb="962" eb="963">
+      <t>gei'ding</t>
+    </rPh>
+    <rPh sb="965" eb="966">
+      <t>jing'xiang</t>
+    </rPh>
+    <rPh sb="968" eb="969">
+      <t>chuang'jian</t>
+    </rPh>
+    <rPh sb="971" eb="972">
+      <t>rong'qi</t>
+    </rPh>
+    <rPh sb="974" eb="975">
+      <t>ying'she</t>
+    </rPh>
+    <rPh sb="976" eb="977">
+      <t>duan'kou</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stage6</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jenkins</t>
+    <rPh sb="0" eb="1">
+      <t>li'yong</t>
+    </rPh>
+    <rPh sb="962" eb="963">
+      <t>gei'ding</t>
+    </rPh>
+    <rPh sb="965" eb="966">
+      <t>jing'xiang</t>
+    </rPh>
+    <rPh sb="968" eb="969">
+      <t>chuang'jian</t>
+    </rPh>
+    <rPh sb="971" eb="972">
+      <t>rong'qi</t>
+    </rPh>
+    <rPh sb="974" eb="975">
+      <t>ying'she</t>
+    </rPh>
+    <rPh sb="976" eb="977">
+      <t>duan'kou</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>jenkins</t>
+  </si>
+  <si>
+    <t>true</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">8080:8080 </t>
+  </si>
+  <si>
+    <t>50000:50000</t>
+  </si>
+  <si>
+    <t>/srv/docker/redmine/redmine:/home/redmine/data</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/srv/docker/jenkins:/var/jenkins_home</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="15"/>
       <color indexed="8"/>
@@ -467,8 +840,14 @@
       <name val="兰亭黑-简 中黑"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="兰亭黑-简 特黑"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="20">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -581,6 +960,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF92CDDC"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -4114,7 +4499,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -4180,9 +4565,6 @@
     <xf numFmtId="49" fontId="14" fillId="6" borderId="1" xfId="1133" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="6" borderId="1" xfId="1133" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="1133" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -4192,50 +4574,64 @@
     <xf numFmtId="0" fontId="6" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="2" xfId="1133" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="3" xfId="1133" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="2" xfId="1133" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="3" xfId="1133" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="1133" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1134">
@@ -5761,7 +6157,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -5805,7 +6201,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -5827,7 +6223,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K126"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -5882,11 +6278,11 @@
       <c r="B4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="34" t="str">
+      <c r="C4" s="37" t="str">
         <f ca="1">REPLACE(CELL("filename"),FIND("[",CELL("filename"))-1,99,)</f>
-        <v>/Users/jiasy/Documents/sourceFrame/excelWorkFlow/excel/dockerContainer</v>
-      </c>
-      <c r="D4" s="35"/>
+        <v>/Users/jiasy/Documents/sourceFrame/pyWorkFlow/excel/dockerContainer</v>
+      </c>
+      <c r="D4" s="38"/>
       <c r="E4" s="3"/>
       <c r="F4" s="1" t="s">
         <v>23</v>
@@ -5896,11 +6292,11 @@
       <c r="B5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="32" t="str">
+      <c r="C5" s="43" t="str">
         <f ca="1">C4&amp;"/../../pythonCode/base/ExcelWorkFlow.py"</f>
-        <v>/Users/jiasy/Documents/sourceFrame/excelWorkFlow/excel/dockerContainer/../../pythonCode/base/ExcelWorkFlow.py</v>
-      </c>
-      <c r="D5" s="32"/>
+        <v>/Users/jiasy/Documents/sourceFrame/pyWorkFlow/excel/dockerContainer/../../pythonCode/base/ExcelWorkFlow.py</v>
+      </c>
+      <c r="D5" s="43"/>
       <c r="E5" s="3"/>
       <c r="F5" s="1" t="s">
         <v>24</v>
@@ -5910,109 +6306,109 @@
       <c r="B6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="32" t="str">
+      <c r="C6" s="43" t="str">
         <f ca="1">C4&amp;"/../../test"</f>
-        <v>/Users/jiasy/Documents/sourceFrame/excelWorkFlow/excel/dockerContainer/../../test</v>
-      </c>
-      <c r="D6" s="36"/>
+        <v>/Users/jiasy/Documents/sourceFrame/pyWorkFlow/excel/dockerContainer/../../test</v>
+      </c>
+      <c r="D6" s="45"/>
       <c r="E6" s="3"/>
     </row>
     <row r="7" spans="2:11" ht="15">
       <c r="B7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="32" t="str">
+      <c r="C7" s="43" t="str">
         <f ca="1">C4&amp;"/../../temp"</f>
-        <v>/Users/jiasy/Documents/sourceFrame/excelWorkFlow/excel/dockerContainer/../../temp</v>
-      </c>
-      <c r="D7" s="33"/>
+        <v>/Users/jiasy/Documents/sourceFrame/pyWorkFlow/excel/dockerContainer/../../temp</v>
+      </c>
+      <c r="D7" s="44"/>
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="2:11" ht="15">
       <c r="B8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="32" t="str">
+      <c r="C8" s="43" t="str">
         <f ca="1">C4&amp;"/../../pythonCode/ClientTools"</f>
-        <v>/Users/jiasy/Documents/sourceFrame/excelWorkFlow/excel/dockerContainer/../../pythonCode/ClientTools</v>
-      </c>
-      <c r="D8" s="33"/>
+        <v>/Users/jiasy/Documents/sourceFrame/pyWorkFlow/excel/dockerContainer/../../pythonCode/ClientTools</v>
+      </c>
+      <c r="D8" s="44"/>
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="2:11" ht="15">
       <c r="B9" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="32" t="str">
+      <c r="C9" s="43" t="str">
         <f ca="1">C4&amp;"/../../pythonCode/ServerTools"</f>
-        <v>/Users/jiasy/Documents/sourceFrame/excelWorkFlow/excel/dockerContainer/../../pythonCode/ServerTools</v>
-      </c>
-      <c r="D9" s="33"/>
+        <v>/Users/jiasy/Documents/sourceFrame/pyWorkFlow/excel/dockerContainer/../../pythonCode/ServerTools</v>
+      </c>
+      <c r="D9" s="44"/>
       <c r="E9" s="3"/>
     </row>
     <row r="10" spans="2:11" ht="15">
       <c r="B10" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="32" t="str">
+      <c r="C10" s="43" t="str">
         <f ca="1">C4&amp;"/../../pythonCode/CommonTools"</f>
-        <v>/Users/jiasy/Documents/sourceFrame/excelWorkFlow/excel/dockerContainer/../../pythonCode/CommonTools</v>
-      </c>
-      <c r="D10" s="33"/>
+        <v>/Users/jiasy/Documents/sourceFrame/pyWorkFlow/excel/dockerContainer/../../pythonCode/CommonTools</v>
+      </c>
+      <c r="D10" s="44"/>
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="2:11" ht="15">
       <c r="B11" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="30" t="str">
+      <c r="C11" s="29" t="str">
         <f ca="1">MID(CELL("filename"),SEARCH("[",CELL("filename"))+1, SEARCH("]",CELL("filename"))-SEARCH("[",CELL("filename"))-1)</f>
         <v>baseDockerContainer.xlsx</v>
       </c>
-      <c r="D11" s="31"/>
+      <c r="D11" s="30"/>
       <c r="E11" s="3"/>
     </row>
     <row r="12" spans="2:11" ht="15">
       <c r="B12" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="30" t="str">
+      <c r="C12" s="29" t="str">
         <f ca="1">MID(CELL("filename"),SEARCH("[",CELL("filename"))+1, SEARCH(".xlsx",CELL("filename"))-SEARCH("[",CELL("filename"))-1)</f>
         <v>baseDockerContainer</v>
       </c>
-      <c r="D12" s="31"/>
+      <c r="D12" s="30"/>
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="2:11" ht="15">
       <c r="B13" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="34" t="str">
+      <c r="C13" s="37" t="str">
         <f ca="1">RIGHT(CELL("filename"),LEN(CELL("filename"))-FIND("]",CELL("filename")))</f>
         <v>pngTest</v>
       </c>
-      <c r="D13" s="35"/>
+      <c r="D13" s="38"/>
       <c r="E13" s="3"/>
     </row>
     <row r="14" spans="2:11" ht="15">
       <c r="B14" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="43" t="str">
+      <c r="C14" s="39" t="str">
         <f ca="1">C4&amp;"/"&amp;C11</f>
-        <v>/Users/jiasy/Documents/sourceFrame/excelWorkFlow/excel/dockerContainer/baseDockerContainer.xlsx</v>
-      </c>
-      <c r="D14" s="44"/>
+        <v>/Users/jiasy/Documents/sourceFrame/pyWorkFlow/excel/dockerContainer/baseDockerContainer.xlsx</v>
+      </c>
+      <c r="D14" s="40"/>
       <c r="E14" s="3"/>
     </row>
     <row r="15" spans="2:11" ht="15">
       <c r="B15" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="38"/>
+      <c r="D15" s="32"/>
       <c r="E15" s="3"/>
       <c r="F15" s="1" t="s">
         <v>22</v>
@@ -6022,21 +6418,21 @@
       <c r="B16" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="37" t="s">
+      <c r="C16" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="38"/>
+      <c r="D16" s="32"/>
       <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:6" ht="15">
       <c r="B17" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="45" t="str">
+      <c r="C17" s="41" t="str">
         <f ca="1">"python "&amp;C5&amp;" -e "&amp;C14</f>
-        <v>python /Users/jiasy/Documents/sourceFrame/excelWorkFlow/excel/dockerContainer/../../pythonCode/base/ExcelWorkFlow.py -e /Users/jiasy/Documents/sourceFrame/excelWorkFlow/excel/dockerContainer/baseDockerContainer.xlsx</v>
-      </c>
-      <c r="D17" s="46"/>
+        <v>python /Users/jiasy/Documents/sourceFrame/pyWorkFlow/excel/dockerContainer/../../pythonCode/base/ExcelWorkFlow.py -e /Users/jiasy/Documents/sourceFrame/pyWorkFlow/excel/dockerContainer/baseDockerContainer.xlsx</v>
+      </c>
+      <c r="D17" s="42"/>
       <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:6" ht="15">
@@ -6058,109 +6454,1036 @@
       <c r="B20" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="40"/>
+      <c r="C20" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="34"/>
       <c r="E20" s="18"/>
       <c r="F20" s="19"/>
     </row>
     <row r="21" spans="1:6" ht="25" customHeight="1" thickBot="1">
       <c r="A21" s="20" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="41" t="str">
+        <v>29</v>
+      </c>
+      <c r="C21" s="35" t="str">
         <f ca="1">C9&amp;"/docker/CreateContainer.py"</f>
-        <v>/Users/jiasy/Documents/sourceFrame/excelWorkFlow/excel/dockerContainer/../../pythonCode/ServerTools/docker/CreateContainer.py</v>
-      </c>
-      <c r="D21" s="42"/>
+        <v>/Users/jiasy/Documents/sourceFrame/pyWorkFlow/excel/dockerContainer/../../pythonCode/ServerTools/docker/CreateContainer.py</v>
+      </c>
+      <c r="D21" s="36"/>
       <c r="E21" s="18"/>
       <c r="F21" s="19"/>
     </row>
     <row r="22" spans="1:6" ht="25" customHeight="1" thickBot="1">
       <c r="A22" s="22"/>
       <c r="B22" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="24" t="s">
+      <c r="D22" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="25" t="s">
+      <c r="E22" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="E22" s="18" t="s">
-        <v>34</v>
-      </c>
       <c r="F22" s="19" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="25" customHeight="1" thickBot="1">
       <c r="A23" s="26"/>
       <c r="B23" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="D23" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="24" t="s">
+      <c r="F23" s="19"/>
+    </row>
+    <row r="24" spans="1:6" ht="25" customHeight="1" thickBot="1">
+      <c r="B24" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="27" t="s">
+      <c r="C24" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="E23" s="18" t="s">
+      <c r="D24" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24" s="18"/>
+    </row>
+    <row r="25" spans="1:6" ht="25" customHeight="1" thickBot="1">
+      <c r="B25" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="28"/>
+      <c r="E25" s="18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="25" customHeight="1" thickBot="1">
+      <c r="B26" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="28"/>
+      <c r="E26" s="18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="25" customHeight="1" thickBot="1">
+      <c r="B27" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" s="47" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="25" customHeight="1" thickBot="1">
+      <c r="B28" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="25" customHeight="1" thickBot="1">
+      <c r="B29" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="F23" s="19"/>
-    </row>
-    <row r="24" spans="1:6" ht="25" customHeight="1" thickBot="1">
-      <c r="A24" s="26"/>
-      <c r="B24" s="23" t="s">
+      <c r="D29" s="47" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="25" customHeight="1" thickBot="1">
+      <c r="B30" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D30" s="47" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="25" customHeight="1" thickBot="1">
+      <c r="A31" s="50"/>
+      <c r="B31" s="50"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="51"/>
+    </row>
+    <row r="32" spans="1:6" ht="25" customHeight="1" thickBot="1">
+      <c r="A32" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" s="34"/>
+      <c r="E32" s="46" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="25" customHeight="1" thickBot="1">
+      <c r="A33" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="35" t="str">
+        <f ca="1">C9&amp;"/docker/CreateContainer.py"</f>
+        <v>/Users/jiasy/Documents/sourceFrame/pyWorkFlow/excel/dockerContainer/../../pythonCode/ServerTools/docker/CreateContainer.py</v>
+      </c>
+      <c r="D33" s="36"/>
+    </row>
+    <row r="34" spans="1:6" ht="25" customHeight="1" thickBot="1">
+      <c r="A34" s="22"/>
+      <c r="B34" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D34" s="28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="25" customHeight="1" thickBot="1">
+      <c r="A35" s="26"/>
+      <c r="B35" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="D35" s="28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="25" customHeight="1" thickBot="1">
+      <c r="B36" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" s="28"/>
+    </row>
+    <row r="37" spans="1:6" ht="25" customHeight="1" thickBot="1">
+      <c r="B37" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C37" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="D37" s="28"/>
+    </row>
+    <row r="38" spans="1:6" ht="25" customHeight="1" thickBot="1">
+      <c r="B38" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C38" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D38" s="28"/>
+    </row>
+    <row r="39" spans="1:6" ht="25" customHeight="1" thickBot="1">
+      <c r="B39" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C39" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D39" s="28"/>
+    </row>
+    <row r="40" spans="1:6" ht="25" customHeight="1" thickBot="1">
+      <c r="B40" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C40" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="24" t="s">
+      <c r="D40" s="28"/>
+    </row>
+    <row r="41" spans="1:6" ht="25" customHeight="1" thickBot="1">
+      <c r="B41" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C41" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D41" s="28" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="25" customHeight="1" thickBot="1">
+      <c r="B42" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="28" t="s">
+      <c r="C42" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D42" s="28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="25" customHeight="1" thickBot="1">
+      <c r="D43" s="28" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="25" customHeight="1" thickBot="1">
+      <c r="D44" s="28" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="25" customHeight="1" thickBot="1">
+      <c r="D45" s="28" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="25" customHeight="1" thickBot="1">
+      <c r="F46" s="2"/>
+    </row>
+    <row r="47" spans="1:6" ht="25" customHeight="1" thickBot="1">
+      <c r="A47" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B47" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C47" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="D47" s="34"/>
+    </row>
+    <row r="48" spans="1:6" ht="25" customHeight="1" thickBot="1">
+      <c r="A48" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B48" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C48" s="35" t="str">
+        <f ca="1">C9&amp;"/docker/CreateContainer.py"</f>
+        <v>/Users/jiasy/Documents/sourceFrame/pyWorkFlow/excel/dockerContainer/../../pythonCode/ServerTools/docker/CreateContainer.py</v>
+      </c>
+      <c r="D48" s="36"/>
+    </row>
+    <row r="49" spans="1:8" ht="25" customHeight="1" thickBot="1">
+      <c r="A49" s="22"/>
+      <c r="B49" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C49" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D49" s="28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="25" customHeight="1" thickBot="1">
+      <c r="A50" s="26"/>
+      <c r="B50" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C50" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="D50" s="28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="25" customHeight="1" thickBot="1">
+      <c r="B51" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C51" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D51" s="28"/>
+    </row>
+    <row r="52" spans="1:8" ht="25" customHeight="1" thickBot="1">
+      <c r="B52" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C52" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D52" s="28"/>
+    </row>
+    <row r="53" spans="1:8" ht="25" customHeight="1" thickBot="1">
+      <c r="B53" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D53" s="28"/>
+    </row>
+    <row r="54" spans="1:8" ht="25" customHeight="1" thickBot="1">
+      <c r="B54" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C54" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D54" s="28"/>
+    </row>
+    <row r="55" spans="1:8" ht="25" customHeight="1" thickBot="1">
+      <c r="B55" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C55" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D55" s="28"/>
+    </row>
+    <row r="56" spans="1:8" ht="25" customHeight="1" thickBot="1">
+      <c r="B56" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="E24" s="18"/>
-      <c r="F24" s="19" t="s">
+      <c r="C56" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D56" s="28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="25" customHeight="1" thickBot="1">
+      <c r="B57" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C57" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D57" s="28"/>
+    </row>
+    <row r="58" spans="1:8" ht="25" customHeight="1" thickBot="1">
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+    </row>
+    <row r="59" spans="1:8" ht="25" customHeight="1" thickBot="1">
+      <c r="A59" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B59" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C59" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="D59" s="34"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+    </row>
+    <row r="60" spans="1:8" ht="25" customHeight="1" thickBot="1">
+      <c r="A60" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B60" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C60" s="35" t="str">
+        <f ca="1">C9&amp;"/docker/CreateContainer.py"</f>
+        <v>/Users/jiasy/Documents/sourceFrame/pyWorkFlow/excel/dockerContainer/../../pythonCode/ServerTools/docker/CreateContainer.py</v>
+      </c>
+      <c r="D60" s="36"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+    </row>
+    <row r="61" spans="1:8" ht="25" customHeight="1" thickBot="1">
+      <c r="A61" s="22"/>
+      <c r="B61" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C61" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D61" s="28" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="25" customHeight="1" thickBot="1">
+      <c r="A62" s="26"/>
+      <c r="B62" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C62" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="D62" s="28" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="25" customHeight="1" thickBot="1">
+      <c r="B63" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C63" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D63" s="28"/>
+    </row>
+    <row r="64" spans="1:8" ht="25" customHeight="1" thickBot="1">
+      <c r="B64" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C64" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D64" s="28"/>
+    </row>
+    <row r="65" spans="1:5" ht="25" customHeight="1" thickBot="1">
+      <c r="B65" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C65" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D65" s="28"/>
+    </row>
+    <row r="66" spans="1:5" ht="25" customHeight="1" thickBot="1">
+      <c r="B66" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C66" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D66" s="28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="25" customHeight="1" thickBot="1">
+      <c r="C67" s="1"/>
+      <c r="D67" s="28" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="25" customHeight="1" thickBot="1">
+      <c r="B68" s="23" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" ht="25" customHeight="1" thickBot="1">
-      <c r="A25" s="26"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="28" t="s">
+      <c r="C68" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D68" s="28" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="25" customHeight="1" thickBot="1">
+      <c r="C69" s="1"/>
+      <c r="D69" s="28" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="25" customHeight="1" thickBot="1">
+      <c r="B70" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C70" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D70" s="28" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="25" customHeight="1" thickBot="1">
+      <c r="B71" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C71" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D71" s="28" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="25" customHeight="1" thickBot="1">
+      <c r="D72" s="28" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="25" customHeight="1" thickBot="1">
+      <c r="D73" s="28" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="25" customHeight="1" thickBot="1">
+      <c r="D74" s="28" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="25" customHeight="1" thickBot="1">
+      <c r="D75" s="28" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="25" customHeight="1" thickBot="1">
+      <c r="A76" s="48"/>
+      <c r="B76" s="48"/>
+      <c r="C76" s="49"/>
+      <c r="D76" s="49"/>
+      <c r="E76" s="49"/>
+    </row>
+    <row r="77" spans="1:5" ht="25" customHeight="1" thickBot="1">
+      <c r="A77" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B77" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C77" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="D77" s="34"/>
+    </row>
+    <row r="78" spans="1:5" ht="25" customHeight="1" thickBot="1">
+      <c r="A78" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B78" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C78" s="35" t="str">
+        <f ca="1">C9&amp;"/docker/CreateContainer.py"</f>
+        <v>/Users/jiasy/Documents/sourceFrame/pyWorkFlow/excel/dockerContainer/../../pythonCode/ServerTools/docker/CreateContainer.py</v>
+      </c>
+      <c r="D78" s="36"/>
+    </row>
+    <row r="79" spans="1:5" ht="25" customHeight="1" thickBot="1">
+      <c r="A79" s="22"/>
+      <c r="B79" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C79" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D79" s="28" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="25" customHeight="1" thickBot="1">
+      <c r="A80" s="26"/>
+      <c r="B80" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C80" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="D80" s="28" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="25" customHeight="1" thickBot="1">
+      <c r="B81" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C81" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D81" s="28"/>
+    </row>
+    <row r="82" spans="1:4" ht="25" customHeight="1" thickBot="1">
+      <c r="B82" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="E25" s="18"/>
-      <c r="F25" s="19" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="25" customHeight="1" thickBot="1">
-      <c r="A26" s="26"/>
-      <c r="B26" s="23" t="s">
+      <c r="C82" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="C26" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="D26" s="29" t="str">
-        <f ca="1">C6&amp;"../../temp/dockerShare:/macShare"</f>
-        <v>/Users/jiasy/Documents/sourceFrame/excelWorkFlow/excel/dockerContainer/../../test../../temp/dockerShare:/macShare</v>
-      </c>
-      <c r="E26" s="18"/>
-      <c r="F26" s="19" t="s">
+      <c r="D82" s="28"/>
+    </row>
+    <row r="83" spans="1:4" ht="25" customHeight="1" thickBot="1">
+      <c r="B83" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C83" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D83" s="28"/>
+    </row>
+    <row r="84" spans="1:4" ht="25" customHeight="1" thickBot="1">
+      <c r="B84" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C84" s="24" t="s">
         <v>48</v>
       </c>
+      <c r="D84" s="28"/>
+    </row>
+    <row r="85" spans="1:4" ht="25" customHeight="1" thickBot="1">
+      <c r="B85" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C85" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D85" s="28"/>
+    </row>
+    <row r="86" spans="1:4" ht="25" customHeight="1" thickBot="1">
+      <c r="B86" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C86" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D86" s="28" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="25" customHeight="1" thickBot="1">
+      <c r="B87" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C87" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D87" s="28" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="25" customHeight="1" thickBot="1">
+      <c r="D88" s="28" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="25" customHeight="1" thickBot="1">
+      <c r="D89" s="28" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="25" customHeight="1" thickBot="1"/>
+    <row r="91" spans="1:4" ht="25" customHeight="1" thickBot="1">
+      <c r="A91" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B91" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C91" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="D91" s="34"/>
+    </row>
+    <row r="92" spans="1:4" ht="25" customHeight="1" thickBot="1">
+      <c r="A92" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B92" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C92" s="35" t="str">
+        <f ca="1">C9&amp;"/docker/CreateContainer.py"</f>
+        <v>/Users/jiasy/Documents/sourceFrame/pyWorkFlow/excel/dockerContainer/../../pythonCode/ServerTools/docker/CreateContainer.py</v>
+      </c>
+      <c r="D92" s="36"/>
+    </row>
+    <row r="93" spans="1:4" ht="25" customHeight="1" thickBot="1">
+      <c r="A93" s="22"/>
+      <c r="B93" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C93" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D93" s="28" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="25" customHeight="1" thickBot="1">
+      <c r="A94" s="26"/>
+      <c r="B94" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C94" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="D94" s="28" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="25" customHeight="1" thickBot="1">
+      <c r="B95" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C95" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D95" s="28"/>
+    </row>
+    <row r="96" spans="1:4" ht="25" customHeight="1" thickBot="1">
+      <c r="B96" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C96" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D96" s="28"/>
+    </row>
+    <row r="97" spans="1:5" ht="25" customHeight="1" thickBot="1">
+      <c r="B97" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C97" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D97" s="28"/>
+    </row>
+    <row r="98" spans="1:5" ht="25" customHeight="1" thickBot="1">
+      <c r="B98" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C98" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D98" s="28" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="25" customHeight="1" thickBot="1">
+      <c r="B99" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C99" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D99" s="28" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="25" customHeight="1" thickBot="1">
+      <c r="B100" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C100" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D100" s="28" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="25" customHeight="1" thickBot="1">
+      <c r="B101" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C101" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D101" s="28" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="25" customHeight="1" thickBot="1">
+      <c r="A102" s="48"/>
+      <c r="B102" s="48"/>
+      <c r="C102" s="49"/>
+      <c r="D102" s="49"/>
+      <c r="E102" s="49"/>
+    </row>
+    <row r="103" spans="1:5" ht="25" customHeight="1" thickBot="1">
+      <c r="A103" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="B103" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C103" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="D103" s="34"/>
+    </row>
+    <row r="104" spans="1:5" ht="25" customHeight="1" thickBot="1">
+      <c r="A104" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B104" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C104" s="35" t="str">
+        <f ca="1">C9&amp;"/docker/CreateContainer.py"</f>
+        <v>/Users/jiasy/Documents/sourceFrame/pyWorkFlow/excel/dockerContainer/../../pythonCode/ServerTools/docker/CreateContainer.py</v>
+      </c>
+      <c r="D104" s="36"/>
+    </row>
+    <row r="105" spans="1:5" ht="25" customHeight="1" thickBot="1">
+      <c r="A105" s="22"/>
+      <c r="B105" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C105" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D105" s="28" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="25" customHeight="1" thickBot="1">
+      <c r="A106" s="26"/>
+      <c r="B106" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C106" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="D106" s="28" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="25" customHeight="1" thickBot="1">
+      <c r="B107" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C107" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D107" s="28"/>
+    </row>
+    <row r="108" spans="1:5" ht="25" customHeight="1" thickBot="1">
+      <c r="B108" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C108" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D108" s="28"/>
+    </row>
+    <row r="109" spans="1:5" ht="25" customHeight="1" thickBot="1">
+      <c r="B109" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C109" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D109" s="28" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="25" customHeight="1" thickBot="1">
+      <c r="B110" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C110" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D110" s="28"/>
+    </row>
+    <row r="111" spans="1:5" ht="25" customHeight="1" thickBot="1">
+      <c r="B111" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C111" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D111" s="28" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="25" customHeight="1" thickBot="1">
+      <c r="C112" s="1"/>
+      <c r="D112" s="28" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="25" customHeight="1" thickBot="1">
+      <c r="B113" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C113" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D113" s="28" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="25" customHeight="1" thickBot="1">
+      <c r="B114" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C114" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D114" s="28"/>
+    </row>
+    <row r="116" spans="1:5" ht="25" customHeight="1">
+      <c r="A116" s="2"/>
+      <c r="C116" s="1"/>
+      <c r="D116" s="1"/>
+      <c r="E116" s="1"/>
+    </row>
+    <row r="117" spans="1:5" ht="25" customHeight="1">
+      <c r="A117" s="2"/>
+      <c r="C117" s="1"/>
+      <c r="D117" s="1"/>
+      <c r="E117" s="1"/>
+    </row>
+    <row r="118" spans="1:5" ht="25" customHeight="1">
+      <c r="A118" s="2"/>
+      <c r="C118" s="1"/>
+      <c r="D118" s="1"/>
+      <c r="E118" s="1"/>
+    </row>
+    <row r="119" spans="1:5" ht="25" customHeight="1">
+      <c r="A119" s="2"/>
+      <c r="C119" s="1"/>
+      <c r="D119" s="1"/>
+      <c r="E119" s="1"/>
+    </row>
+    <row r="120" spans="1:5" ht="25" customHeight="1">
+      <c r="A120" s="2"/>
+      <c r="C120" s="1"/>
+      <c r="D120" s="1"/>
+      <c r="E120" s="1"/>
+    </row>
+    <row r="121" spans="1:5" ht="25" customHeight="1">
+      <c r="A121" s="2"/>
+      <c r="C121" s="1"/>
+      <c r="D121" s="1"/>
+      <c r="E121" s="1"/>
+    </row>
+    <row r="122" spans="1:5" ht="25" customHeight="1">
+      <c r="A122" s="2"/>
+      <c r="C122" s="1"/>
+      <c r="D122" s="1"/>
+      <c r="E122" s="1"/>
+    </row>
+    <row r="123" spans="1:5" ht="25" customHeight="1">
+      <c r="A123" s="2"/>
+      <c r="C123" s="1"/>
+      <c r="D123" s="1"/>
+      <c r="E123" s="1"/>
+    </row>
+    <row r="124" spans="1:5" ht="25" customHeight="1">
+      <c r="A124" s="2"/>
+      <c r="C124" s="1"/>
+      <c r="D124" s="1"/>
+      <c r="E124" s="1"/>
+    </row>
+    <row r="125" spans="1:5" ht="25" customHeight="1">
+      <c r="A125" s="2"/>
+      <c r="C125" s="1"/>
+      <c r="D125" s="1"/>
+      <c r="E125" s="1"/>
+    </row>
+    <row r="126" spans="1:5" ht="25" customHeight="1">
+      <c r="A126" s="2"/>
+      <c r="C126" s="1"/>
+      <c r="D126" s="1"/>
+      <c r="E126" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="28">
+    <mergeCell ref="C103:D103"/>
+    <mergeCell ref="C104:D104"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C8:D8"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="C20:D20"/>
@@ -6169,22 +7492,14 @@
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C8:D8"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2">
       <formula1>J2:J4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A21">
-      <formula1>J4:J5</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A21 A33 A48 A60 A78 A92 A104">
+      <formula1>$J$2:$J$3</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777779102325439" footer="0.27777779102325439"/>

</xml_diff>

<commit_message>
修改 ServerTools/docker/CreateContainer 添加 net 可选参数，添加 excel/dockerContainer/openresty.xlsx 支持openresty的docker run 添加 CommonTools/File/FileFilterByRegs.py 为拷贝的升级版，通过后缀指定拷贝类型，通过正则表达式去掉不想拷贝的内容。 修改CommonTools/Jenkins/ExcuteWorkFlowByExcel.py ,可以不填写jenkins替换参数。 添加 CommonTools/Json/addIndexToElements.py 用来为列表类的json文件的每一个元素添加一个序号 【待完善】 添加 CommonTools/Code/jsLogTrail.py 用来做js的代码方法输出，简单版本，展示没有堆栈显示【待完善】 添加 CommonTools/Code/luaLogTrailTemplet/LogTrailUtilForBaseLua.lua 一个lua使用log工具，不是Cocos2dx 写法的通用lua文件。 添加 excel/code/luaTestLogTrail.xlsx ，用来对lua文件夹内的代码进行log附加，用于小文件夹。
</commit_message>
<xml_diff>
--- a/excel/dockerContainer/baseDockerContainer.xlsx
+++ b/excel/dockerContainer/baseDockerContainer.xlsx
@@ -18,6 +18,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">pngTest!#REF!</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -333,7 +334,7 @@
   </si>
   <si>
     <t>名称:版本</t>
-    <rPh sb="0" eb="13">
+    <rPh sb="0" eb="5">
       <t>min'bheng</t>
     </rPh>
     <phoneticPr fontId="13" type="noConversion"/>
@@ -355,25 +356,7 @@
   <si>
     <t>运行容器设置模板，注意左侧Stage1下面的off，这样使得它不会被执行</t>
     <rPh sb="0" eb="1">
-      <t>li'yong</t>
-    </rPh>
-    <rPh sb="570" eb="571">
-      <t>gei'ding</t>
-    </rPh>
-    <rPh sb="573" eb="574">
-      <t>jing'xiang</t>
-    </rPh>
-    <rPh sb="576" eb="577">
-      <t>chuang'jian</t>
-    </rPh>
-    <rPh sb="579" eb="580">
-      <t>rong'qi</t>
-    </rPh>
-    <rPh sb="582" eb="583">
-      <t>ying'she</t>
-    </rPh>
-    <rPh sb="584" eb="585">
-      <t>duan'kou</t>
+      <t>li'yonggei'dingjing'xiangchuang'jianrong'qiying'sheduan'kou</t>
     </rPh>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -427,25 +410,7 @@
   <si>
     <t>GitLab搭建第一步，sql容器</t>
     <rPh sb="0" eb="1">
-      <t>li'yong</t>
-    </rPh>
-    <rPh sb="728" eb="729">
-      <t>gei'ding</t>
-    </rPh>
-    <rPh sb="731" eb="732">
-      <t>jing'xiang</t>
-    </rPh>
-    <rPh sb="734" eb="735">
-      <t>chuang'jian</t>
-    </rPh>
-    <rPh sb="737" eb="738">
-      <t>rong'qi</t>
-    </rPh>
-    <rPh sb="740" eb="741">
-      <t>ying'she</t>
-    </rPh>
-    <rPh sb="742" eb="743">
-      <t>duan'kou</t>
+      <t>li'yonggei'dingjing'xiangchuang'jianrong'qiying'sheduan'kou</t>
     </rPh>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -476,7 +441,7 @@
   </si>
   <si>
     <t>两边双引号有程序添加，这里就写值</t>
-    <rPh sb="0" eb="485">
+    <rPh sb="0" eb="16">
       <t>yin'hao</t>
     </rPh>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -509,50 +474,14 @@
   <si>
     <t>GitLab搭建第二步，redis容器</t>
     <rPh sb="0" eb="1">
-      <t>li'yong</t>
-    </rPh>
-    <rPh sb="825" eb="826">
-      <t>gei'ding</t>
-    </rPh>
-    <rPh sb="828" eb="829">
-      <t>jing'xiang</t>
-    </rPh>
-    <rPh sb="831" eb="832">
-      <t>chuang'jian</t>
-    </rPh>
-    <rPh sb="834" eb="835">
-      <t>rong'qi</t>
-    </rPh>
-    <rPh sb="837" eb="838">
-      <t>ying'she</t>
-    </rPh>
-    <rPh sb="839" eb="840">
-      <t>duan'kou</t>
+      <t>li'yonggei'dingjing'xiangchuang'jianrong'qiying'sheduan'kou</t>
     </rPh>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>GitLab搭建第三步，gitlab</t>
     <rPh sb="0" eb="1">
-      <t>li'yong</t>
-    </rPh>
-    <rPh sb="841" eb="842">
-      <t>gei'ding</t>
-    </rPh>
-    <rPh sb="844" eb="845">
-      <t>jing'xiang</t>
-    </rPh>
-    <rPh sb="847" eb="848">
-      <t>chuang'jian</t>
-    </rPh>
-    <rPh sb="850" eb="851">
-      <t>rong'qi</t>
-    </rPh>
-    <rPh sb="853" eb="854">
-      <t>ying'she</t>
-    </rPh>
-    <rPh sb="855" eb="856">
-      <t>duan'kou</t>
+      <t>li'yonggei'dingjing'xiangchuang'jianrong'qiying'sheduan'kou</t>
     </rPh>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -598,7 +527,7 @@
   </si>
   <si>
     <t>最好先下载镜像，否则会比较慢</t>
-    <rPh sb="0" eb="299">
+    <rPh sb="0" eb="14">
       <t>dai'mai</t>
     </rPh>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -614,25 +543,7 @@
   <si>
     <t>Redmine搭建第一步，SQL</t>
     <rPh sb="0" eb="1">
-      <t>li'yong</t>
-    </rPh>
-    <rPh sb="918" eb="919">
-      <t>gei'ding</t>
-    </rPh>
-    <rPh sb="921" eb="922">
-      <t>jing'xiang</t>
-    </rPh>
-    <rPh sb="924" eb="925">
-      <t>chuang'jian</t>
-    </rPh>
-    <rPh sb="927" eb="928">
-      <t>rong'qi</t>
-    </rPh>
-    <rPh sb="930" eb="931">
-      <t>ying'she</t>
-    </rPh>
-    <rPh sb="932" eb="933">
-      <t>duan'kou</t>
+      <t>li'yonggei'dingjing'xiangchuang'jianrong'qiying'sheduan'kou</t>
     </rPh>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -670,25 +581,7 @@
   <si>
     <t>Redmine搭建第二步，Redmine</t>
     <rPh sb="0" eb="1">
-      <t>li'yong</t>
-    </rPh>
-    <rPh sb="962" eb="963">
-      <t>gei'ding</t>
-    </rPh>
-    <rPh sb="965" eb="966">
-      <t>jing'xiang</t>
-    </rPh>
-    <rPh sb="968" eb="969">
-      <t>chuang'jian</t>
-    </rPh>
-    <rPh sb="971" eb="972">
-      <t>rong'qi</t>
-    </rPh>
-    <rPh sb="974" eb="975">
-      <t>ying'she</t>
-    </rPh>
-    <rPh sb="976" eb="977">
-      <t>duan'kou</t>
+      <t>li'yonggei'dingjing'xiangchuang'jianrong'qiying'sheduan'kou</t>
     </rPh>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -699,25 +592,7 @@
   <si>
     <t>Jenkins</t>
     <rPh sb="0" eb="1">
-      <t>li'yong</t>
-    </rPh>
-    <rPh sb="962" eb="963">
-      <t>gei'ding</t>
-    </rPh>
-    <rPh sb="965" eb="966">
-      <t>jing'xiang</t>
-    </rPh>
-    <rPh sb="968" eb="969">
-      <t>chuang'jian</t>
-    </rPh>
-    <rPh sb="971" eb="972">
-      <t>rong'qi</t>
-    </rPh>
-    <rPh sb="974" eb="975">
-      <t>ying'she</t>
-    </rPh>
-    <rPh sb="976" eb="977">
-      <t>duan'kou</t>
+      <t>li'yonggei'dingjing'xiangchuang'jianrong'qiying'sheduan'kou</t>
     </rPh>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -4568,57 +4443,6 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="1133" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="2" xfId="1133" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="3" xfId="1133" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -4632,6 +4456,57 @@
     <xf numFmtId="0" fontId="5" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="2" xfId="1133" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="3" xfId="1133" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1134">
@@ -6157,7 +6032,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -6201,7 +6076,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -6278,11 +6153,11 @@
       <c r="B4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="37" t="str">
+      <c r="C4" s="43" t="str">
         <f ca="1">REPLACE(CELL("filename"),FIND("[",CELL("filename"))-1,99,)</f>
         <v>/Users/jiasy/Documents/sourceFrame/pyWorkFlow/excel/dockerContainer</v>
       </c>
-      <c r="D4" s="38"/>
+      <c r="D4" s="44"/>
       <c r="E4" s="3"/>
       <c r="F4" s="1" t="s">
         <v>23</v>
@@ -6292,11 +6167,11 @@
       <c r="B5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="43" t="str">
+      <c r="C5" s="41" t="str">
         <f ca="1">C4&amp;"/../../pythonCode/base/ExcelWorkFlow.py"</f>
         <v>/Users/jiasy/Documents/sourceFrame/pyWorkFlow/excel/dockerContainer/../../pythonCode/base/ExcelWorkFlow.py</v>
       </c>
-      <c r="D5" s="43"/>
+      <c r="D5" s="41"/>
       <c r="E5" s="3"/>
       <c r="F5" s="1" t="s">
         <v>24</v>
@@ -6306,7 +6181,7 @@
       <c r="B6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="43" t="str">
+      <c r="C6" s="41" t="str">
         <f ca="1">C4&amp;"/../../test"</f>
         <v>/Users/jiasy/Documents/sourceFrame/pyWorkFlow/excel/dockerContainer/../../test</v>
       </c>
@@ -6317,98 +6192,98 @@
       <c r="B7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="43" t="str">
+      <c r="C7" s="41" t="str">
         <f ca="1">C4&amp;"/../../temp"</f>
         <v>/Users/jiasy/Documents/sourceFrame/pyWorkFlow/excel/dockerContainer/../../temp</v>
       </c>
-      <c r="D7" s="44"/>
+      <c r="D7" s="42"/>
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="2:11" ht="15">
       <c r="B8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="43" t="str">
+      <c r="C8" s="41" t="str">
         <f ca="1">C4&amp;"/../../pythonCode/ClientTools"</f>
         <v>/Users/jiasy/Documents/sourceFrame/pyWorkFlow/excel/dockerContainer/../../pythonCode/ClientTools</v>
       </c>
-      <c r="D8" s="44"/>
+      <c r="D8" s="42"/>
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="2:11" ht="15">
       <c r="B9" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="43" t="str">
+      <c r="C9" s="41" t="str">
         <f ca="1">C4&amp;"/../../pythonCode/ServerTools"</f>
         <v>/Users/jiasy/Documents/sourceFrame/pyWorkFlow/excel/dockerContainer/../../pythonCode/ServerTools</v>
       </c>
-      <c r="D9" s="44"/>
+      <c r="D9" s="42"/>
       <c r="E9" s="3"/>
     </row>
     <row r="10" spans="2:11" ht="15">
       <c r="B10" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="43" t="str">
+      <c r="C10" s="41" t="str">
         <f ca="1">C4&amp;"/../../pythonCode/CommonTools"</f>
         <v>/Users/jiasy/Documents/sourceFrame/pyWorkFlow/excel/dockerContainer/../../pythonCode/CommonTools</v>
       </c>
-      <c r="D10" s="44"/>
+      <c r="D10" s="42"/>
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="2:11" ht="15">
       <c r="B11" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="29" t="str">
+      <c r="C11" s="39" t="str">
         <f ca="1">MID(CELL("filename"),SEARCH("[",CELL("filename"))+1, SEARCH("]",CELL("filename"))-SEARCH("[",CELL("filename"))-1)</f>
         <v>baseDockerContainer.xlsx</v>
       </c>
-      <c r="D11" s="30"/>
+      <c r="D11" s="40"/>
       <c r="E11" s="3"/>
     </row>
     <row r="12" spans="2:11" ht="15">
       <c r="B12" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="29" t="str">
+      <c r="C12" s="39" t="str">
         <f ca="1">MID(CELL("filename"),SEARCH("[",CELL("filename"))+1, SEARCH(".xlsx",CELL("filename"))-SEARCH("[",CELL("filename"))-1)</f>
         <v>baseDockerContainer</v>
       </c>
-      <c r="D12" s="30"/>
+      <c r="D12" s="40"/>
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="2:11" ht="15">
       <c r="B13" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="37" t="str">
+      <c r="C13" s="43" t="str">
         <f ca="1">RIGHT(CELL("filename"),LEN(CELL("filename"))-FIND("]",CELL("filename")))</f>
         <v>pngTest</v>
       </c>
-      <c r="D13" s="38"/>
+      <c r="D13" s="44"/>
       <c r="E13" s="3"/>
     </row>
     <row r="14" spans="2:11" ht="15">
       <c r="B14" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="39" t="str">
+      <c r="C14" s="48" t="str">
         <f ca="1">C4&amp;"/"&amp;C11</f>
         <v>/Users/jiasy/Documents/sourceFrame/pyWorkFlow/excel/dockerContainer/baseDockerContainer.xlsx</v>
       </c>
-      <c r="D14" s="40"/>
+      <c r="D14" s="49"/>
       <c r="E14" s="3"/>
     </row>
     <row r="15" spans="2:11" ht="15">
       <c r="B15" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="31" t="s">
+      <c r="C15" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="32"/>
+      <c r="D15" s="47"/>
       <c r="E15" s="3"/>
       <c r="F15" s="1" t="s">
         <v>22</v>
@@ -6418,21 +6293,21 @@
       <c r="B16" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="32"/>
+      <c r="D16" s="47"/>
       <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:6" ht="15">
       <c r="B17" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="41" t="str">
+      <c r="C17" s="50" t="str">
         <f ca="1">"python "&amp;C5&amp;" -e "&amp;C14</f>
         <v>python /Users/jiasy/Documents/sourceFrame/pyWorkFlow/excel/dockerContainer/../../pythonCode/base/ExcelWorkFlow.py -e /Users/jiasy/Documents/sourceFrame/pyWorkFlow/excel/dockerContainer/baseDockerContainer.xlsx</v>
       </c>
-      <c r="D17" s="42"/>
+      <c r="D17" s="51"/>
       <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:6" ht="15">
@@ -6454,10 +6329,10 @@
       <c r="B20" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="33" t="s">
+      <c r="C20" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="34"/>
+      <c r="D20" s="36"/>
       <c r="E20" s="18"/>
       <c r="F20" s="19"/>
     </row>
@@ -6468,11 +6343,11 @@
       <c r="B21" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="35" t="str">
+      <c r="C21" s="37" t="str">
         <f ca="1">C9&amp;"/docker/CreateContainer.py"</f>
         <v>/Users/jiasy/Documents/sourceFrame/pyWorkFlow/excel/dockerContainer/../../pythonCode/ServerTools/docker/CreateContainer.py</v>
       </c>
-      <c r="D21" s="36"/>
+      <c r="D21" s="38"/>
       <c r="E21" s="18"/>
       <c r="F21" s="19"/>
     </row>
@@ -6517,7 +6392,7 @@
       <c r="C24" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="47" t="s">
+      <c r="D24" s="30" t="s">
         <v>55</v>
       </c>
       <c r="E24" s="18"/>
@@ -6553,7 +6428,7 @@
       <c r="C27" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="D27" s="47" t="s">
+      <c r="D27" s="30" t="s">
         <v>54</v>
       </c>
     </row>
@@ -6575,7 +6450,7 @@
       <c r="C29" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D29" s="47" t="s">
+      <c r="D29" s="30" t="s">
         <v>52</v>
       </c>
     </row>
@@ -6586,16 +6461,16 @@
       <c r="C30" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="D30" s="47" t="s">
+      <c r="D30" s="30" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="25" customHeight="1" thickBot="1">
-      <c r="A31" s="50"/>
-      <c r="B31" s="50"/>
-      <c r="C31" s="51"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="51"/>
+      <c r="A31" s="33"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34"/>
     </row>
     <row r="32" spans="1:6" ht="25" customHeight="1" thickBot="1">
       <c r="A32" s="16" t="s">
@@ -6604,11 +6479,11 @@
       <c r="B32" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="33" t="s">
+      <c r="C32" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="D32" s="34"/>
-      <c r="E32" s="46" t="s">
+      <c r="D32" s="36"/>
+      <c r="E32" s="29" t="s">
         <v>90</v>
       </c>
     </row>
@@ -6619,11 +6494,11 @@
       <c r="B33" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="35" t="str">
+      <c r="C33" s="37" t="str">
         <f ca="1">C9&amp;"/docker/CreateContainer.py"</f>
         <v>/Users/jiasy/Documents/sourceFrame/pyWorkFlow/excel/dockerContainer/../../pythonCode/ServerTools/docker/CreateContainer.py</v>
       </c>
-      <c r="D33" s="36"/>
+      <c r="D33" s="38"/>
     </row>
     <row r="34" spans="1:6" ht="25" customHeight="1" thickBot="1">
       <c r="A34" s="22"/>
@@ -6741,10 +6616,10 @@
       <c r="B47" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C47" s="33" t="s">
+      <c r="C47" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="D47" s="34"/>
+      <c r="D47" s="36"/>
     </row>
     <row r="48" spans="1:6" ht="25" customHeight="1" thickBot="1">
       <c r="A48" s="20" t="s">
@@ -6753,11 +6628,11 @@
       <c r="B48" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C48" s="35" t="str">
+      <c r="C48" s="37" t="str">
         <f ca="1">C9&amp;"/docker/CreateContainer.py"</f>
         <v>/Users/jiasy/Documents/sourceFrame/pyWorkFlow/excel/dockerContainer/../../pythonCode/ServerTools/docker/CreateContainer.py</v>
       </c>
-      <c r="D48" s="36"/>
+      <c r="D48" s="38"/>
     </row>
     <row r="49" spans="1:8" ht="25" customHeight="1" thickBot="1">
       <c r="A49" s="22"/>
@@ -6860,10 +6735,10 @@
       <c r="B59" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C59" s="33" t="s">
+      <c r="C59" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="D59" s="34"/>
+      <c r="D59" s="36"/>
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
@@ -6875,11 +6750,11 @@
       <c r="B60" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C60" s="35" t="str">
+      <c r="C60" s="37" t="str">
         <f ca="1">C9&amp;"/docker/CreateContainer.py"</f>
         <v>/Users/jiasy/Documents/sourceFrame/pyWorkFlow/excel/dockerContainer/../../pythonCode/ServerTools/docker/CreateContainer.py</v>
       </c>
-      <c r="D60" s="36"/>
+      <c r="D60" s="38"/>
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
@@ -7012,11 +6887,11 @@
       </c>
     </row>
     <row r="76" spans="1:5" ht="25" customHeight="1" thickBot="1">
-      <c r="A76" s="48"/>
-      <c r="B76" s="48"/>
-      <c r="C76" s="49"/>
-      <c r="D76" s="49"/>
-      <c r="E76" s="49"/>
+      <c r="A76" s="31"/>
+      <c r="B76" s="31"/>
+      <c r="C76" s="32"/>
+      <c r="D76" s="32"/>
+      <c r="E76" s="32"/>
     </row>
     <row r="77" spans="1:5" ht="25" customHeight="1" thickBot="1">
       <c r="A77" s="16" t="s">
@@ -7025,10 +6900,10 @@
       <c r="B77" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C77" s="33" t="s">
+      <c r="C77" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="D77" s="34"/>
+      <c r="D77" s="36"/>
     </row>
     <row r="78" spans="1:5" ht="25" customHeight="1" thickBot="1">
       <c r="A78" s="20" t="s">
@@ -7037,11 +6912,11 @@
       <c r="B78" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C78" s="35" t="str">
+      <c r="C78" s="37" t="str">
         <f ca="1">C9&amp;"/docker/CreateContainer.py"</f>
         <v>/Users/jiasy/Documents/sourceFrame/pyWorkFlow/excel/dockerContainer/../../pythonCode/ServerTools/docker/CreateContainer.py</v>
       </c>
-      <c r="D78" s="36"/>
+      <c r="D78" s="38"/>
     </row>
     <row r="79" spans="1:5" ht="25" customHeight="1" thickBot="1">
       <c r="A79" s="22"/>
@@ -7152,10 +7027,10 @@
       <c r="B91" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C91" s="33" t="s">
+      <c r="C91" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="D91" s="34"/>
+      <c r="D91" s="36"/>
     </row>
     <row r="92" spans="1:4" ht="25" customHeight="1" thickBot="1">
       <c r="A92" s="20" t="s">
@@ -7164,11 +7039,11 @@
       <c r="B92" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C92" s="35" t="str">
+      <c r="C92" s="37" t="str">
         <f ca="1">C9&amp;"/docker/CreateContainer.py"</f>
         <v>/Users/jiasy/Documents/sourceFrame/pyWorkFlow/excel/dockerContainer/../../pythonCode/ServerTools/docker/CreateContainer.py</v>
       </c>
-      <c r="D92" s="36"/>
+      <c r="D92" s="38"/>
     </row>
     <row r="93" spans="1:4" ht="25" customHeight="1" thickBot="1">
       <c r="A93" s="22"/>
@@ -7266,11 +7141,11 @@
       </c>
     </row>
     <row r="102" spans="1:5" ht="25" customHeight="1" thickBot="1">
-      <c r="A102" s="48"/>
-      <c r="B102" s="48"/>
-      <c r="C102" s="49"/>
-      <c r="D102" s="49"/>
-      <c r="E102" s="49"/>
+      <c r="A102" s="31"/>
+      <c r="B102" s="31"/>
+      <c r="C102" s="32"/>
+      <c r="D102" s="32"/>
+      <c r="E102" s="32"/>
     </row>
     <row r="103" spans="1:5" ht="25" customHeight="1" thickBot="1">
       <c r="A103" s="16" t="s">
@@ -7279,10 +7154,10 @@
       <c r="B103" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C103" s="33" t="s">
+      <c r="C103" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="D103" s="34"/>
+      <c r="D103" s="36"/>
     </row>
     <row r="104" spans="1:5" ht="25" customHeight="1" thickBot="1">
       <c r="A104" s="20" t="s">
@@ -7291,11 +7166,11 @@
       <c r="B104" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C104" s="35" t="str">
+      <c r="C104" s="37" t="str">
         <f ca="1">C9&amp;"/docker/CreateContainer.py"</f>
         <v>/Users/jiasy/Documents/sourceFrame/pyWorkFlow/excel/dockerContainer/../../pythonCode/ServerTools/docker/CreateContainer.py</v>
       </c>
-      <c r="D104" s="36"/>
+      <c r="D104" s="38"/>
     </row>
     <row r="105" spans="1:5" ht="25" customHeight="1" thickBot="1">
       <c r="A105" s="22"/>
@@ -7464,18 +7339,14 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="C103:D103"/>
-    <mergeCell ref="C104:D104"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C10:D10"/>
@@ -7484,14 +7355,18 @@
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C103:D103"/>
+    <mergeCell ref="C104:D104"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="C92:D92"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="2">

</xml_diff>